<commit_message>
Handle NotImplementedExpection for subtotal formulas (SHEET-307) vaadin/spreadsheet#404
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_Invalid_formula.xlsx
+++ b/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_Invalid_formula.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guille/Projects/spreadsheet/vaadin-spreadsheet/src/test/resources/test_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11085"/>
+    <workbookView xWindow="0" yWindow="1340" windowWidth="28800" windowHeight="11080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="150001" calcMode="manual" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,18 +30,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Grain</t>
   </si>
   <si>
     <t>Fooo</t>
   </si>
+  <si>
+    <t>cell with formula  condition</t>
+  </si>
+  <si>
+    <t>cell with formula value and &gt; condition</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
@@ -89,7 +101,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -115,9 +157,56 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -431,15 +520,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -447,16 +539,62 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
+      <c r="F1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f>SUBTOTAL(109,F1:F5)</f>
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="thisMonth">
+    <cfRule type="timePeriod" dxfId="8" priority="4" timePeriod="thisMonth">
       <formula>AND(MONTH(A1)=MONTH(TODAY()),YEAR(A1)=YEAR(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Grain">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Grain">
       <formula>NOT(ISERROR(SEARCH("Grain",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThan">
+      <formula>$B$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$B$3&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>